<commit_message>
now able to show the differences of two Excel sheets
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RequirementsAnalysis\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orlando/Desktop/RequirementsAnalysis/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B05490-DFB8-4419-A6BC-B3567EFF0B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B89A540-19DA-0B40-85A7-5925A8881B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
   <si>
     <t>Data B1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -97,23 +97,29 @@
   <si>
     <t>h4</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data Ds</t>
+  </si>
+  <si>
+    <t>h5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -154,7 +160,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -434,13 +440,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -452,7 +458,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -466,7 +472,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
@@ -482,7 +488,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -500,7 +506,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -518,7 +524,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -536,7 +542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -553,7 +559,6 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
@@ -562,6 +567,7 @@
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -570,15 +576,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBCE0DF6-166D-424E-B7B2-2F0B72819E43}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:F7"/>
+    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -590,7 +596,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -604,7 +610,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
@@ -620,7 +626,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -638,7 +644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -653,10 +659,10 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -674,7 +680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -689,8 +695,27 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>

</xml_diff>